<commit_message>
vendordetail controller and model added
</commit_message>
<xml_diff>
--- a/DataDictionaryOLS.xlsx
+++ b/DataDictionaryOLS.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmallProjectsInt\onlineLocalService\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
   <si>
     <t>Sr. No. 1</t>
   </si>
@@ -181,9 +189,6 @@
     <t>ServiceDetails</t>
   </si>
   <si>
-    <t>serviceDetailId</t>
-  </si>
-  <si>
     <t>pk</t>
   </si>
   <si>
@@ -212,24 +217,35 @@
   </si>
   <si>
     <t xml:space="preserve">foreign key </t>
+  </si>
+  <si>
+    <t>A Table that shows vendor details</t>
+  </si>
+  <si>
+    <t>a vendor must have a userId, availability, price, more info about his service, with also a subcategory id that shows its category</t>
+  </si>
+  <si>
+    <t>subcat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -239,54 +255,55 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -476,33 +493,38 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A3:F75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="34.57"/>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -519,7 +541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -527,13 +549,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -541,13 +563,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="4">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -558,17 +580,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -585,7 +607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -593,13 +615,13 @@
         <v>19</v>
       </c>
       <c r="C13" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -607,13 +629,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="4">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -621,7 +643,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>21</v>
@@ -630,7 +652,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -641,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -649,10 +671,10 @@
         <v>11</v>
       </c>
       <c r="C17" s="4">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -660,29 +682,29 @@
         <v>11</v>
       </c>
       <c r="C18" s="4">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -699,7 +721,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
@@ -707,13 +729,13 @@
         <v>19</v>
       </c>
       <c r="C25" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
@@ -721,13 +743,13 @@
         <v>11</v>
       </c>
       <c r="C26" s="4">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
@@ -735,17 +757,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
@@ -762,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -770,13 +792,13 @@
         <v>8</v>
       </c>
       <c r="C33" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
@@ -784,10 +806,10 @@
         <v>11</v>
       </c>
       <c r="C34" s="4">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -795,7 +817,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>21</v>
@@ -804,7 +826,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>13</v>
       </c>
@@ -812,12 +834,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>36</v>
       </c>
@@ -826,7 +848,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -843,7 +865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>37</v>
       </c>
@@ -851,13 +873,13 @@
         <v>8</v>
       </c>
       <c r="C41" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>18</v>
       </c>
@@ -865,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>21</v>
@@ -874,7 +896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>39</v>
       </c>
@@ -882,10 +904,10 @@
         <v>11</v>
       </c>
       <c r="C43" s="4">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>40</v>
       </c>
@@ -893,25 +915,25 @@
         <v>8</v>
       </c>
       <c r="C44" s="4">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>2</v>
       </c>
@@ -928,7 +950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>44</v>
       </c>
@@ -936,13 +958,13 @@
         <v>19</v>
       </c>
       <c r="C50" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>18</v>
       </c>
@@ -950,7 +972,7 @@
         <v>19</v>
       </c>
       <c r="C51" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>21</v>
@@ -962,7 +984,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
@@ -970,7 +992,7 @@
         <v>19</v>
       </c>
       <c r="C52" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>21</v>
@@ -979,7 +1001,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>37</v>
       </c>
@@ -987,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="C53" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>21</v>
@@ -996,7 +1018,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>13</v>
       </c>
@@ -1004,17 +1026,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="58">
+      <c r="B57" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>2</v>
       </c>
@@ -1031,7 +1059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>51</v>
       </c>
@@ -1039,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>21</v>
@@ -1048,7 +1076,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>52</v>
       </c>
@@ -1056,10 +1084,10 @@
         <v>53</v>
       </c>
       <c r="C60" s="4">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>54</v>
       </c>
@@ -1067,10 +1095,10 @@
         <v>8</v>
       </c>
       <c r="C61" s="4">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>55</v>
       </c>
@@ -1078,42 +1106,45 @@
         <v>11</v>
       </c>
       <c r="C62" s="4">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="4">
+        <v>9</v>
+      </c>
+      <c r="D63" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C63" s="4">
-        <v>9.0</v>
-      </c>
-      <c r="D63" s="4" t="s">
+      <c r="E63" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="4" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>2</v>
       </c>
@@ -1130,29 +1161,29 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="4">
+        <v>9</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="4">
-        <v>9.0</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="B71" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>21</v>
@@ -1161,15 +1192,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C72" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>21</v>
@@ -1178,32 +1209,32 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C73" s="4">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>51</v>
       </c>
@@ -1211,13 +1242,13 @@
         <v>8</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>